<commit_message>
fix(hw/sch): fix led and R5
</commit_message>
<xml_diff>
--- a/hardware/array/daplink_array_JLCSMT.xlsx
+++ b/hardware/array/daplink_array_JLCSMT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andy\Desktop\DAPLink\hardware\daplink\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andy\Desktop\DAPLink\hardware\array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E725EE-4823-45B3-AC05-B2204C78A5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD91A7F-737A-494C-9376-C079F425184A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10695" yWindow="1290" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="81">
   <si>
     <t>Comment</t>
   </si>
@@ -294,12 +294,15 @@
   <si>
     <t>C115962</t>
   </si>
+  <si>
+    <t>C22775</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -335,6 +338,19 @@
       <name val="細明體"/>
       <family val="3"/>
       <charset val="136"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -374,7 +390,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -389,6 +405,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -733,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -962,7 +984,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -976,7 +998,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -990,7 +1012,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1004,7 +1026,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1018,7 +1040,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -1032,9 +1054,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A22" t="s">
-        <v>15</v>
+    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A22" s="5">
+        <v>100</v>
       </c>
       <c r="B22" t="s">
         <v>60</v>
@@ -1042,11 +1064,12 @@
       <c r="C22" t="s">
         <v>35</v>
       </c>
-      <c r="D22" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="D22" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -1060,7 +1083,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -1074,7 +1097,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A25">
         <v>470</v>
       </c>
@@ -1088,7 +1111,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1102,7 +1125,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="27" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -1116,7 +1139,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="28" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1130,7 +1153,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="29" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A29">
         <v>33</v>
       </c>
@@ -1144,7 +1167,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="30" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A30">
         <v>33</v>
       </c>
@@ -1158,7 +1181,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="31" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -1169,7 +1192,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A32" t="s">
         <v>18</v>
       </c>

</xml_diff>